<commit_message>
add new dxf elements: ARC and LINE
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>6.79</t>
+          <t>0.64</t>
         </is>
       </c>
     </row>
@@ -534,7 +534,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>3.45</t>
+          <t>0.34</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>27.15</t>
+          <t>2.56</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>40.48</t>
+          <t>3.76</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>10.12</t>
+          <t>0.94</t>
         </is>
       </c>
     </row>
@@ -658,7 +658,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>40.48</t>
+          <t>3.76</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>20.24</t>
+          <t>1.88</t>
         </is>
       </c>
     </row>

</xml_diff>